<commit_message>
cambios para probar en la pc de arriba
</commit_message>
<xml_diff>
--- a/Estrategias_Optimas.xlsx
+++ b/Estrategias_Optimas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,94 +472,163 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" t="n">
         <v>150</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
-        <v>552000</v>
+        <v>69400</v>
       </c>
       <c r="G2" t="n">
-        <v>0.411122211122211</v>
+        <v>0.2164772727272727</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="n">
         <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3" t="n">
         <v>150</v>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
-        <v>570000</v>
+        <v>63200</v>
       </c>
       <c r="G3" t="n">
-        <v>0.4060606060606061</v>
+        <v>0.2145833333333333</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="n">
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4" t="n">
         <v>100</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" t="n">
-        <v>909000</v>
+        <v>170200</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3987820512820512</v>
+        <v>0.1921882832080201</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" t="n">
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D5" t="n">
+        <v>100</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" t="n">
+        <v>151800</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.1890533625730994</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="n">
+        <v>8</v>
+      </c>
+      <c r="D6" t="n">
         <v>150</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E6" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" t="n">
+        <v>59400</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.1770021645021645</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" t="n">
         <v>5</v>
       </c>
-      <c r="F5" t="n">
-        <v>537000</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.3958225108225109</v>
+      <c r="C7" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" t="n">
+        <v>150</v>
+      </c>
+      <c r="E7" t="n">
+        <v>4</v>
+      </c>
+      <c r="F7" t="n">
+        <v>113800</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.30625</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" t="n">
+        <v>150</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4</v>
+      </c>
+      <c r="F8" t="n">
+        <v>90200</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.250297619047619</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
confirmar todos los cambios finalizado
</commit_message>
<xml_diff>
--- a/Estrategias_Optimas.xlsx
+++ b/Estrategias_Optimas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -631,6 +631,75 @@
         <v>0.250297619047619</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="n">
+        <v>12</v>
+      </c>
+      <c r="C9" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" t="n">
+        <v>150</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4</v>
+      </c>
+      <c r="F9" t="n">
+        <v>574200</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.6767144892144892</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" t="n">
+        <v>12</v>
+      </c>
+      <c r="C10" t="n">
+        <v>4</v>
+      </c>
+      <c r="D10" t="n">
+        <v>200</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" t="n">
+        <v>574200</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.6767144892144892</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" t="n">
+        <v>12</v>
+      </c>
+      <c r="C11" t="n">
+        <v>4</v>
+      </c>
+      <c r="D11" t="n">
+        <v>250</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4</v>
+      </c>
+      <c r="F11" t="n">
+        <v>574200</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.6767144892144892</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
probando numeros anteriores con 9
</commit_message>
<xml_diff>
--- a/Estrategias_Optimas.xlsx
+++ b/Estrategias_Optimas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,22 +475,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="E2" t="n">
         <v>4</v>
       </c>
       <c r="F2" t="n">
-        <v>69400</v>
+        <v>23000</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2164772727272727</v>
+        <v>0.04040085616235199</v>
       </c>
     </row>
     <row r="3">
@@ -498,22 +498,22 @@
         <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E3" t="n">
         <v>4</v>
       </c>
       <c r="F3" t="n">
-        <v>63200</v>
+        <v>45000</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2145833333333333</v>
+        <v>0.09766834365325078</v>
       </c>
     </row>
     <row r="4">
@@ -521,22 +521,22 @@
         <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E4" t="n">
         <v>4</v>
       </c>
       <c r="F4" t="n">
-        <v>170200</v>
+        <v>66400</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1921882832080201</v>
+        <v>0.1056810634474137</v>
       </c>
     </row>
     <row r="5">
@@ -547,19 +547,19 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D5" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E5" t="n">
         <v>4</v>
       </c>
       <c r="F5" t="n">
-        <v>151800</v>
+        <v>69400</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1890533625730994</v>
+        <v>0.2164772727272727</v>
       </c>
     </row>
     <row r="6">
@@ -570,7 +570,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6" t="n">
         <v>150</v>
@@ -579,10 +579,10 @@
         <v>4</v>
       </c>
       <c r="F6" t="n">
-        <v>59400</v>
+        <v>63200</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1770021645021645</v>
+        <v>0.2145833333333333</v>
       </c>
     </row>
     <row r="7">
@@ -590,22 +590,22 @@
         <v>0</v>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" t="n">
         <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E7" t="n">
         <v>4</v>
       </c>
       <c r="F7" t="n">
-        <v>113800</v>
+        <v>170200</v>
       </c>
       <c r="G7" t="n">
-        <v>0.30625</v>
+        <v>0.1921882832080201</v>
       </c>
     </row>
     <row r="8">
@@ -613,33 +613,33 @@
         <v>0</v>
       </c>
       <c r="B8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" t="n">
         <v>5</v>
       </c>
       <c r="D8" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E8" t="n">
         <v>4</v>
       </c>
       <c r="F8" t="n">
-        <v>90200</v>
+        <v>151800</v>
       </c>
       <c r="G8" t="n">
-        <v>0.250297619047619</v>
+        <v>0.1890533625730994</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D9" t="n">
         <v>150</v>
@@ -648,56 +648,286 @@
         <v>4</v>
       </c>
       <c r="F9" t="n">
-        <v>574200</v>
+        <v>59400</v>
       </c>
       <c r="G9" t="n">
-        <v>0.6767144892144892</v>
+        <v>0.1770021645021645</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B10" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C10" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D10" t="n">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E10" t="n">
         <v>4</v>
       </c>
       <c r="F10" t="n">
-        <v>574200</v>
+        <v>113800</v>
       </c>
       <c r="G10" t="n">
-        <v>0.6767144892144892</v>
+        <v>0.30625</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11" t="n">
+        <v>5</v>
+      </c>
+      <c r="C11" t="n">
+        <v>5</v>
+      </c>
+      <c r="D11" t="n">
+        <v>150</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4</v>
+      </c>
+      <c r="F11" t="n">
+        <v>90200</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.250297619047619</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>0</v>
+      </c>
+      <c r="B12" t="n">
+        <v>5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" t="n">
+        <v>50</v>
+      </c>
+      <c r="E12" t="n">
+        <v>4</v>
+      </c>
+      <c r="F12" t="n">
+        <v>125800</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.1605156679822188</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" t="n">
+        <v>100</v>
+      </c>
+      <c r="E13" t="n">
+        <v>4</v>
+      </c>
+      <c r="F13" t="n">
+        <v>19800</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.1806308049535604</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" t="n">
+        <v>4</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" t="n">
+        <v>100</v>
+      </c>
+      <c r="E14" t="n">
+        <v>4</v>
+      </c>
+      <c r="F14" t="n">
+        <v>84600</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.3441057394617766</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" t="n">
+        <v>5</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" t="n">
+        <v>100</v>
+      </c>
+      <c r="E15" t="n">
+        <v>4</v>
+      </c>
+      <c r="F15" t="n">
+        <v>94800</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.4059061681352703</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" t="n">
         <v>12</v>
       </c>
-      <c r="C11" t="n">
-        <v>4</v>
-      </c>
-      <c r="D11" t="n">
+      <c r="C16" t="n">
+        <v>4</v>
+      </c>
+      <c r="D16" t="n">
+        <v>150</v>
+      </c>
+      <c r="E16" t="n">
+        <v>4</v>
+      </c>
+      <c r="F16" t="n">
+        <v>574200</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.6767144892144892</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1</v>
+      </c>
+      <c r="B17" t="n">
+        <v>12</v>
+      </c>
+      <c r="C17" t="n">
+        <v>4</v>
+      </c>
+      <c r="D17" t="n">
+        <v>200</v>
+      </c>
+      <c r="E17" t="n">
+        <v>4</v>
+      </c>
+      <c r="F17" t="n">
+        <v>574200</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.6767144892144892</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1</v>
+      </c>
+      <c r="B18" t="n">
+        <v>12</v>
+      </c>
+      <c r="C18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D18" t="n">
         <v>250</v>
       </c>
-      <c r="E11" t="n">
-        <v>4</v>
-      </c>
-      <c r="F11" t="n">
+      <c r="E18" t="n">
+        <v>4</v>
+      </c>
+      <c r="F18" t="n">
         <v>574200</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G18" t="n">
         <v>0.6767144892144892</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" t="n">
+        <v>12</v>
+      </c>
+      <c r="C19" t="n">
+        <v>5</v>
+      </c>
+      <c r="D19" t="n">
+        <v>150</v>
+      </c>
+      <c r="E19" t="n">
+        <v>4</v>
+      </c>
+      <c r="F19" t="n">
+        <v>639600</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.6724780701754386</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" t="n">
+        <v>12</v>
+      </c>
+      <c r="C20" t="n">
+        <v>5</v>
+      </c>
+      <c r="D20" t="n">
+        <v>200</v>
+      </c>
+      <c r="E20" t="n">
+        <v>4</v>
+      </c>
+      <c r="F20" t="n">
+        <v>639600</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.6724780701754386</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" t="n">
+        <v>12</v>
+      </c>
+      <c r="C21" t="n">
+        <v>5</v>
+      </c>
+      <c r="D21" t="n">
+        <v>250</v>
+      </c>
+      <c r="E21" t="n">
+        <v>4</v>
+      </c>
+      <c r="F21" t="n">
+        <v>639600</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.6724780701754386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>